<commit_message>
Successfuly scheduled data with only one week, needs more testing
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,15 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D19CQDT03-B + D19CQDT04-B  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">D19CQDT01-B + D19CQDT02-B   </t>
   </si>
 </sst>
 </file>
@@ -413,12 +407,6 @@
       <c r="A2">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">

</xml_diff>

<commit_message>
Translated and added support for dates
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,9 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Day</t>
+  </si>
+  <si>
+    <t>19/9</t>
+  </si>
+  <si>
+    <t>20/9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D19CQDT03-B + D19CQDT04-B  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">D19CQDT01-B + D19CQDT02-B   </t>
   </si>
 </sst>
 </file>
@@ -404,13 +416,19 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2">
-        <v>5</v>
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3">
-        <v>3</v>
+      <c r="A3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>